<commit_message>
machine_operation_timeline 시계열 데이터 시각화
</commit_message>
<xml_diff>
--- a/results/trace.xlsx
+++ b/results/trace.xlsx
@@ -88,10 +88,10 @@
     <t>M1-&gt;M2</t>
   </si>
   <si>
+    <t>M3</t>
+  </si>
+  <si>
     <t>M2</t>
-  </si>
-  <si>
-    <t>M3</t>
   </si>
   <si>
     <t>M3-&gt;M1</t>
@@ -597,7 +597,7 @@
         <v>30</v>
       </c>
       <c r="F5">
-        <v>2.497388159546499</v>
+        <v>3.607996782156957</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -617,10 +617,10 @@
         <v>31</v>
       </c>
       <c r="F6">
-        <v>2.497388159546499</v>
+        <v>3.607996782156957</v>
       </c>
       <c r="I6">
-        <v>1.240697716423126</v>
+        <v>1.668701124354598</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -640,7 +640,7 @@
         <v>29</v>
       </c>
       <c r="F7">
-        <v>2.497388159546499</v>
+        <v>3.607996782156957</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -648,13 +648,13 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
         <v>24</v>
@@ -663,24 +663,24 @@
         <v>28</v>
       </c>
       <c r="F8">
-        <v>3.738085875969624</v>
+        <v>4</v>
       </c>
       <c r="G8">
         <v>1</v>
       </c>
       <c r="H8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
         <v>24</v>
@@ -689,7 +689,7 @@
         <v>29</v>
       </c>
       <c r="F9">
-        <v>3.738085875969624</v>
+        <v>4</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -697,13 +697,13 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D10" t="s">
         <v>25</v>
@@ -712,24 +712,24 @@
         <v>28</v>
       </c>
       <c r="F10">
-        <v>4</v>
+        <v>5.276697906511554</v>
       </c>
       <c r="G10">
         <v>1</v>
       </c>
       <c r="H10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D11" t="s">
         <v>25</v>
@@ -738,7 +738,7 @@
         <v>29</v>
       </c>
       <c r="F11">
-        <v>4</v>
+        <v>5.276697906511554</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -761,7 +761,7 @@
         <v>30</v>
       </c>
       <c r="F12">
-        <v>5.38273722185208</v>
+        <v>6.702257725566692</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -781,30 +781,36 @@
         <v>31</v>
       </c>
       <c r="F13">
-        <v>5.38273722185208</v>
+        <v>6.702257725566692</v>
       </c>
       <c r="I13">
-        <v>1.672460823119295</v>
+        <v>1.7191080394563</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D14" t="s">
         <v>25</v>
       </c>
       <c r="E14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F14">
-        <v>6.185150365070152</v>
+        <v>8.421365765022992</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -815,157 +821,151 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F15">
-        <v>6.185150365070152</v>
-      </c>
-      <c r="I15">
-        <v>1.434679070691841</v>
+        <v>9.457171722217414</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D16" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E16" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F16">
-        <v>7.055198044971375</v>
-      </c>
-      <c r="G16">
-        <v>1</v>
-      </c>
-      <c r="H16" t="s">
-        <v>19</v>
+        <v>9.457171722217414</v>
+      </c>
+      <c r="I16">
+        <v>1.690519551256694</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C17" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D17" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E17" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F17">
-        <v>7.619829435761993</v>
-      </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-      <c r="H17" t="s">
-        <v>20</v>
+        <v>10.91628103788027</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C18" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D18" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E18" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F18">
-        <v>7.619829435761993</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
+        <v>10.91628103788027</v>
+      </c>
+      <c r="I18">
+        <v>0.719117402088626</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C19" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D19" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F19">
-        <v>8.220854190739834</v>
+        <v>10.91628103788027</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B20" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D20" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E20" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F20">
-        <v>8.220854190739834</v>
-      </c>
-      <c r="I20">
-        <v>0.9885317110951787</v>
+        <v>11.14769127347411</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C21" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E21" t="s">
         <v>29</v>
       </c>
       <c r="F21">
-        <v>8.220854190739834</v>
+        <v>11.14769127347411</v>
       </c>
       <c r="G21">
         <v>0</v>
@@ -988,7 +988,7 @@
         <v>28</v>
       </c>
       <c r="F22">
-        <v>9.209385901835013</v>
+        <v>11.63539843996889</v>
       </c>
       <c r="G22">
         <v>1</v>
@@ -1014,7 +1014,7 @@
         <v>30</v>
       </c>
       <c r="F23">
-        <v>10.97326315300164</v>
+        <v>14.54747669087936</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -1028,7 +1028,7 @@
         <v>32</v>
       </c>
       <c r="F24">
-        <v>10.97326315300164</v>
+        <v>14.54747669087936</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -1048,7 +1048,7 @@
         <v>29</v>
       </c>
       <c r="F25">
-        <v>10.97326315300164</v>
+        <v>14.54747669087936</v>
       </c>
       <c r="G25">
         <v>0</v>
@@ -1065,13 +1065,13 @@
         <v>19</v>
       </c>
       <c r="D26" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E26" t="s">
         <v>30</v>
       </c>
       <c r="F26">
-        <v>12.31465919648237</v>
+        <v>14.58431033061374</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1085,7 +1085,7 @@
         <v>32</v>
       </c>
       <c r="F27">
-        <v>12.31465919648237</v>
+        <v>14.58431033061374</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -1105,7 +1105,7 @@
         <v>30</v>
       </c>
       <c r="F28">
-        <v>20.50889236677717</v>
+        <v>17.05990858031197</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -1119,7 +1119,7 @@
         <v>32</v>
       </c>
       <c r="F29">
-        <v>20.50889236677717</v>
+        <v>17.05990858031197</v>
       </c>
     </row>
   </sheetData>

</xml_diff>